<commit_message>
Segmentation Paper ICFHR. Images.
</commit_message>
<xml_diff>
--- a/Thesis/Segmentation Paper ICFHR/Segmenattion paper graphs.xlsx
+++ b/Thesis/Segmentation Paper ICFHR/Segmenattion paper graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="475" yWindow="82" windowWidth="27795" windowHeight="12335"/>
+    <workbookView xWindow="475" yWindow="82" windowWidth="7608" windowHeight="5040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -357,8 +357,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="119517568"/>
-        <c:axId val="119519104"/>
+        <c:axId val="247062912"/>
+        <c:axId val="247064448"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -422,11 +422,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119534720"/>
-        <c:axId val="119520640"/>
+        <c:axId val="247481472"/>
+        <c:axId val="247065984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119517568"/>
+        <c:axId val="247062912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,7 +436,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119519104"/>
+        <c:crossAx val="247064448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -444,7 +444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119519104"/>
+        <c:axId val="247064448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.60000000000000009"/>
@@ -456,12 +456,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119517568"/>
+        <c:crossAx val="247062912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119520640"/>
+        <c:axId val="247065984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.30000000000000004"/>
@@ -472,12 +472,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119534720"/>
+        <c:crossAx val="247481472"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="119534720"/>
+        <c:axId val="247481472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,7 +486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119520640"/>
+        <c:crossAx val="247065984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -511,7 +511,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="700"/>
+        <a:defRPr sz="1200"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Segmentation Paper ICFHR - Last version
</commit_message>
<xml_diff>
--- a/Thesis/Segmentation Paper ICFHR/Segmenattion paper graphs.xlsx
+++ b/Thesis/Segmentation Paper ICFHR/Segmenattion paper graphs.xlsx
@@ -21,13 +21,13 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>SR</t>
+    <t>Average WP Segmentation Time [ms]</t>
   </si>
   <si>
-    <t xml:space="preserve"> RR</t>
+    <t>WP SR</t>
   </si>
   <si>
-    <t>Average WP Segmentation Time [ms]</t>
+    <t>WP RR</t>
   </si>
 </sst>
 </file>
@@ -193,7 +193,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SR</c:v>
+                  <c:v>WP SR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -275,7 +275,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> RR</c:v>
+                  <c:v>WP RR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -357,76 +357,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="247062912"/>
-        <c:axId val="247064448"/>
+        <c:axId val="170975616"/>
+        <c:axId val="170977152"/>
       </c:barChart>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Average WP Segmentation Time [ms]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.57699999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.57099999999999995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.59099999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.56599999999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.60799999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.56999999999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="247481472"/>
-        <c:axId val="247065984"/>
-      </c:lineChart>
       <c:catAx>
-        <c:axId val="247062912"/>
+        <c:axId val="170975616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,7 +371,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247064448"/>
+        <c:crossAx val="170977152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -444,7 +379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="247064448"/>
+        <c:axId val="170977152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.60000000000000009"/>
@@ -456,43 +391,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247062912"/>
+        <c:crossAx val="170975616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:valAx>
-        <c:axId val="247065984"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0.30000000000000004"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247481472"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="247481472"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247065984"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
@@ -849,7 +751,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -859,13 +761,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>